<commit_message>
🔄 Actualización automática del mapa (mapa_interactivo_Optical_Power.html)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:P87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4770,7 +4770,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>3715</t>
+          <t>5973</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4780,17 +4780,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>EL SERENO 358</t>
+          <t>PALOS 432</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807168098</t>
+          <t>807168105</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4805,7 +4805,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4813,7 +4813,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4823,30 +4823,30 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.487371</v>
+        <v>-58.362579</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.640099</v>
+        <v>-34.635096</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>5997</t>
+          <t>3715</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4856,17 +4856,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>MARMOL, JOSE 256</t>
+          <t>EL SERENO 358</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807187768</t>
+          <t>807168098</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4881,7 +4881,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Picada coincide con reclamo de cables con mismo numero de caso</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4889,7 +4889,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4899,30 +4899,30 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.425845</v>
+        <v>-58.487371</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.616562</v>
+        <v>-34.640099</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t xml:space="preserve">807187860 </t>
+          <t>5997</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4932,7 +4932,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Av. San Juan 3960</t>
+          <t>MARMOL, JOSE 256</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4942,7 +4942,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807187860</t>
+          <t>807187768</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4957,7 +4957,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Colocar columna contactar a Matias Tapia 1171744701 por si hay alguna duda o problema que surja en el momento ya que es para posterior tendido de ftth</t>
+          <t>Picada coincide con reclamo de cables con mismo numero de caso</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4978,25 +4978,37 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M60" t="inlineStr"/>
-      <c r="N60" t="inlineStr"/>
-      <c r="O60" t="inlineStr"/>
-      <c r="P60" t="inlineStr"/>
+      <c r="M60" t="n">
+        <v>-58.425845</v>
+      </c>
+      <c r="N60" t="n">
+        <v>-34.616562</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6004</t>
+          <t xml:space="preserve">807187860 </t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>MAZA 181</t>
+          <t>San Juan 3960</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -5006,7 +5018,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807215439</t>
+          <t>807187860</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5021,7 +5033,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada coincide con reclamo de cables</t>
+          <t>Colocar columna contactar a Matias Tapia 1171744701 por si hay alguna duda o problema que surja en el momento ya que es para posterior tendido de ftth</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5042,27 +5054,15 @@
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M61" t="n">
-        <v>-58.416477</v>
-      </c>
-      <c r="N61" t="n">
-        <v>-34.61303</v>
-      </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P61" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
+      <c r="M61" t="inlineStr"/>
+      <c r="N61" t="inlineStr"/>
+      <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6007</t>
+          <t>6004</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5072,7 +5072,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>HUMAHUACA 4435</t>
+          <t>MAZA 181</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5082,7 +5082,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807215448</t>
+          <t>807215439</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5119,10 +5119,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.427424</v>
+        <v>-58.416477</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.601217</v>
+        <v>-34.61303</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5138,7 +5138,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6008</t>
+          <t>6007</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5148,7 +5148,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>ESTADO DE ISRAEL AV. 4306</t>
+          <t>HUMAHUACA 4435</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5158,7 +5158,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807215455</t>
+          <t>807215448</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5173,7 +5173,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada coincide con reclamo de cables</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5195,10 +5195,10 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.426665</v>
+        <v>-58.427424</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.598019</v>
+        <v>-34.601217</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5214,7 +5214,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6010</t>
+          <t>6008</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5224,7 +5224,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>ESTADO DE PALESTINA 771</t>
+          <t>ESTADO DE ISRAEL AV. 4306</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -5234,7 +5234,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807215458</t>
+          <t>807215455</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5249,7 +5249,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada y mal ubicada coincide con reclamo de cables</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5271,10 +5271,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.425478</v>
+        <v>-58.426665</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.601865</v>
+        <v>-34.598019</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5290,27 +5290,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6130</t>
+          <t>6010</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 490</t>
+          <t>ESTADO DE PALESTINA 771</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807458227</t>
+          <t>807215458</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5325,7 +5325,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Desmontar columa ya traspasaron un nodo solo falta retirar</t>
+          <t>Picada y mal ubicada coincide con reclamo de cables</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5347,10 +5347,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.440448</v>
+        <v>-58.425478</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.611223</v>
+        <v>-34.601865</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5366,27 +5366,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6168</t>
+          <t>6130</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>ACUÑA DE FIGUEROA, FRANCISCO 566</t>
+          <t>VALLESE, FELIPE 490</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807537512</t>
+          <t>807458227</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5401,7 +5401,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Solo retirar columna tlc coloco una nueva y ya traspsaso sus activos</t>
+          <t>Desmontar columa ya traspasaron un nodo solo falta retirar</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5423,10 +5423,10 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.422775</v>
+        <v>-58.440448</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.604135</v>
+        <v>-34.611223</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -5442,27 +5442,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6214</t>
+          <t>6168</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>GONZALEZ, JOAQUIN V. 2308</t>
+          <t>ACUÑA DE FIGUEROA, FRANCISCO 566</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807605710</t>
+          <t>807537512</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5477,7 +5477,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Solo retirar columna tlc coloco una nueva y ya traspsaso sus activos</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -5495,50 +5495,50 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.497698</v>
+        <v>-58.422775</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.612038</v>
+        <v>-34.604135</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6229</t>
+          <t>6214</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 309</t>
+          <t>GONZALEZ, JOAQUIN V. 2308</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>807762987</t>
+          <t>807605710</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5553,7 +5553,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Reparar rienda </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -5575,26 +5575,26 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.44848</v>
+        <v>-58.497698</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.581338</v>
+        <v>-34.612038</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6228</t>
+          <t>6229</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5604,7 +5604,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE AV. 3416</t>
+          <t>ALVAREZ THOMAS AV. 309</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -5614,7 +5614,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>807762990</t>
+          <t>807762987</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5629,7 +5629,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t xml:space="preserve">Reparar rienda </t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5651,26 +5651,26 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.448496</v>
+        <v>-58.44848</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.58182</v>
+        <v>-34.581338</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6076</t>
+          <t>6228</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5680,17 +5680,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>MATHEU 727</t>
+          <t>NEWBERY, JORGE AV. 3416</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>807763063</t>
+          <t>807762990</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5705,7 +5705,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir a base traspaso de nodo propio y posterior a TLC</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5713,60 +5713,60 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.400169</v>
+        <v>-58.448496</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.617784</v>
+        <v>-34.58182</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6249</t>
+          <t>6076</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>6/25/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>GODOY CRUZ 2696</t>
+          <t>MATHEU 727</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>807789682</t>
+          <t>807763063</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5781,7 +5781,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Inclinada posible cambio</t>
+          <t>Colocar R400 para pedir a base traspaso de nodo propio y posterior a TLC</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5794,7 +5794,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
@@ -5803,14 +5803,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.425296</v>
+        <v>-58.400169</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.578706</v>
+        <v>-34.617784</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5822,27 +5822,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6271</t>
+          <t>6249</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>6/25/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>ARGERICH 740</t>
+          <t>GODOY CRUZ 2696</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>807789686</t>
+          <t>807789682</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5857,7 +5857,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada posible cambio</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5879,46 +5879,46 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.474467</v>
+        <v>-58.425296</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.624161</v>
+        <v>-34.578706</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>-493</t>
+          <t>6271</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>6/27/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>JUFRE 424</t>
+          <t>ARGERICH 740</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>807817955</t>
+          <t>807789686</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5933,7 +5933,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5941,7 +5941,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -5955,46 +5955,46 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.432644</v>
+        <v>-58.474467</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.595434</v>
+        <v>-34.624161</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6284</t>
+          <t>-493</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>6/27/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>CHILE 2561</t>
+          <t>JUFRE 424</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>807851584</t>
+          <t>807817955</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6009,7 +6009,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso</t>
+          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6017,12 +6017,12 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
@@ -6031,14 +6031,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.401827</v>
+        <v>-58.432644</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.617667</v>
+        <v>-34.595434</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6050,27 +6050,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6298</t>
+          <t>6284</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>RIVERA INDARTE AV. 1406</t>
+          <t>CHILE 2561</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>807877127</t>
+          <t>807851584</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6085,7 +6085,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Columna en plantera Se recomienda el retiro riesgo de caida</t>
+          <t>Colocar columna para pedir traspaso</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6098,7 +6098,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
@@ -6107,14 +6107,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.450359</v>
+        <v>-58.401827</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.643582</v>
+        <v>-34.617667</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6126,7 +6126,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6298</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6136,7 +6136,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>RIVERA INDARTE AV. 1406</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -6146,7 +6146,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>807877127</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6161,7 +6161,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Columna con base corroida oxidada</t>
+          <t>Columna en plantera Se recomienda el retiro riesgo de caida</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6183,10 +6183,10 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.459566</v>
+        <v>-58.450359</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.634615</v>
+        <v>-34.643582</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6202,7 +6202,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6308</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6212,17 +6212,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Guayaquil 637</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>807896343</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6237,7 +6237,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna con base corroida oxidada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6259,10 +6259,10 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.437378</v>
+        <v>-58.459566</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.62116</v>
+        <v>-34.634615</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -6278,27 +6278,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6330</t>
+          <t>6308</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>REPUBLICA DE LA INDIA 3106</t>
+          <t>Guayaquil 637</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>807965776</t>
+          <t>807896343</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6313,7 +6313,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada e inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6335,14 +6335,14 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.413941</v>
+        <v>-58.437378</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.57698</v>
+        <v>-34.62116</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6354,7 +6354,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-501</t>
+          <t>6330</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6364,7 +6364,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Cabello 3107</t>
+          <t>REPUBLICA DE LA INDIA 3106</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -6374,7 +6374,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>807971967</t>
+          <t>807965776</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6389,15 +6389,15 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada e inclinada</t>
         </is>
       </c>
       <c r="I79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -6407,18 +6407,18 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.405749</v>
+        <v>-58.413941</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.58224</v>
+        <v>-34.57698</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6430,27 +6430,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6357</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>7/7/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>BACACAY 3088</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808036196</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6465,15 +6465,15 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -6487,26 +6487,26 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.473179</v>
+        <v>-58.405749</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.629138</v>
+        <v>-34.58224</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>-502</t>
+          <t>6357</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6516,17 +6516,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Tagle 2562</t>
+          <t>BACACAY 3088</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>808036198</t>
+          <t>808036196</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6541,7 +6541,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso nodo teco</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6549,60 +6549,60 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.400188</v>
+        <v>-58.473179</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.583882</v>
+        <v>-34.629138</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>-502</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>GUARDIA VIEJA 4377</t>
+          <t>Tagle 2562</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808099347</t>
+          <t>808036198</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6617,7 +6617,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna para pedir traspaso nodo teco</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6630,7 +6630,7 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L82" t="inlineStr">
@@ -6639,14 +6639,14 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.426322</v>
+        <v>-58.400188</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.600097</v>
+        <v>-34.583882</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -6658,7 +6658,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>6383</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -6668,17 +6668,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 1411</t>
+          <t>GUARDIA VIEJA 4377</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808099320</t>
+          <t>808099347</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6715,14 +6715,14 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.448523</v>
+        <v>-58.426322</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.62452</v>
+        <v>-34.600097</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -6734,72 +6734,304 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
+          <t>6383</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>7/8/2025</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>FALCON, RAMON L.,CNEL. 1411</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>808099320</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>-58.448523</v>
+      </c>
+      <c r="N84" t="n">
+        <v>-34.62452</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
           <t>-506</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr">
+      <c r="B85" t="inlineStr">
         <is>
           <t>7/11/2025</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>Gervasio Espinosa 591</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Espinosa 591</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr">
+      <c r="E85" t="inlineStr">
         <is>
           <t>808150511</t>
         </is>
       </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
         <is>
           <t>Picada</t>
         </is>
       </c>
-      <c r="I84" t="n">
-        <v>1</v>
-      </c>
-      <c r="J84" t="inlineStr">
+      <c r="I85" t="n">
+        <v>1</v>
+      </c>
+      <c r="J85" t="inlineStr">
         <is>
           <t>Cambio</t>
         </is>
       </c>
-      <c r="K84" t="inlineStr">
+      <c r="K85" t="inlineStr">
         <is>
           <t>Nodo Teco</t>
         </is>
       </c>
-      <c r="L84" t="inlineStr">
+      <c r="L85" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M84" t="inlineStr"/>
-      <c r="N84" t="inlineStr"/>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>No ubicado</t>
-        </is>
-      </c>
-      <c r="P84" t="inlineStr">
-        <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+      <c r="M85" t="n">
+        <v>-58.449</v>
+      </c>
+      <c r="N85" t="n">
+        <v>-34.616077</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>-511</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>7/14/2025</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Carlos Melo 491</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>808194932</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I86" t="n">
+        <v>1</v>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M86" t="n">
+        <v>-58.363292</v>
+      </c>
+      <c r="N86" t="n">
+        <v>-34.642869</v>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P86" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>-513</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>7/15/2025</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Montes de Oca 1809</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>808240768</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Colocar columna donde esta el monoducto para acceso a edifciio</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M87" t="n">
+        <v>-58.372941</v>
+      </c>
+      <c r="N87" t="n">
+        <v>-34.648341</v>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>